<commit_message>
BOM addition of User Mod for HD12 MGN12
</commit_message>
<xml_diff>
--- a/files/HOTEND_EXTRUDER/RAPIDO/BOM_HextrudORT_Extruder_Rapido.xlsx
+++ b/files/HOTEND_EXTRUDER/RAPIDO/BOM_HextrudORT_Extruder_Rapido.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\RAPIDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDC88A3-6930-4C1E-AE26-034126DC44D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF08969E-8929-4440-A771-6B2C141F9603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="120">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -368,12 +368,6 @@
     <t>Standard fan shroud for Rapido by MirageC</t>
   </si>
   <si>
-    <t>HORTPC_Rapido_HD12_MGN9</t>
-  </si>
-  <si>
-    <t>Rapido Structural Fan Mount HD12</t>
-  </si>
-  <si>
     <t>https://s.click.aliexpress.com/e/_AZtQjU</t>
   </si>
   <si>
@@ -393,9 +387,6 @@
 Aliexpress</t>
   </si>
   <si>
-    <t>HORTPC_RapidoUHF_Spacer HD12_MGN9</t>
-  </si>
-  <si>
     <t>HextrudORT_DRAGON_RAPIDO Body_V1.5</t>
   </si>
   <si>
@@ -411,34 +402,255 @@
     <t>BLTouch support for HD12 RAPIDO UHF</t>
   </si>
   <si>
-    <t>For HextrudORT HD12 Rapido standard.</t>
-  </si>
-  <si>
-    <t>For HextrudORT HD12 Rapido UHF (Ultra High Flow)</t>
-  </si>
-  <si>
-    <t>For HextrudORT HD12 Rapido Standard and High Flow. This fan shroud acts as an additional mouting point for the RAPIDO hotend.</t>
-  </si>
-  <si>
-    <t>RAPIDO UHF spacer for HORTPC HevORT Remote Turbine Part Cooling</t>
-  </si>
-  <si>
     <t>3D Printed (Resin)**</t>
-  </si>
-  <si>
-    <t>HD12 MGN9 Rapido HORTPC - HevORT Remote Turbine Part Cooling
-**Recommended to be printed from SLA (Resin Printer)</t>
   </si>
   <si>
     <t>HextrudORT Rapido / Dragon Tension Arm.
 V1.5 adds some rigidity for better print quality.</t>
+  </si>
+  <si>
+    <t>11C</t>
+  </si>
+  <si>
+    <t>MAKE(Option)</t>
+  </si>
+  <si>
+    <t>11a</t>
+  </si>
+  <si>
+    <t>12b</t>
+  </si>
+  <si>
+    <t>12a</t>
+  </si>
+  <si>
+    <t>13a</t>
+  </si>
+  <si>
+    <t>11b</t>
+  </si>
+  <si>
+    <t>13b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rapido Structural Fan Mount HD12 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MGN9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HORTPC_RapidoUHF_Spacer HD12_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MGN9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HORTPC_Rapido_HD12_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MGN9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For HextrudORT HD12 Rapido Standard and High Flow. This fan shroud acts as an additional mouting point for the RAPIDO hotend.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*For HD12_MGN9</t>
+    </r>
+  </si>
+  <si>
+    <t>MAKE(Option*)</t>
+  </si>
+  <si>
+    <t>*For HextrudORT HD12 Rapido UHF (Ultra High Flow)</t>
+  </si>
+  <si>
+    <t>*For HextrudORT HD12 Rapido standard.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HD12 MGN9 Rapido HORTPC - HevORT Remote Turbine Part Cooling
+**Recommended to be printed from SLA (Resin Printer)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*For HD12_MGN9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RAPIDO UHF spacer for HORTPC HevORT Remote Turbine Part Cooling
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*For HD12_MGN9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HORTPC_RapidoUHF_Spacer HD12_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MGN12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rapido Structural Fan Mount HD12_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MGN12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For HextrudORT HD12 Rapido Standard and High Flow. This fan shroud acts as an additional mouting point for the RAPIDO hotend.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*For HD12_MGN12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HORTPC_Rapido
+HD12_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MGN12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RAPIDO UHF spacer for HORTPC HevORT Remote Turbine Part Cooling
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*For HD12_MGN12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HD12 MGN9 Rapido HORTPC - HevORT Remote Turbine Part Cooling
+**Recommended to be printed from SLA (Resin Printer)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*For HD12_MGN12</t>
+    </r>
+  </si>
+  <si>
+    <t>USER MOD!! Thanks to DonnerPlays from HevORT Discord channel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,6 +793,30 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -766,7 +1002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -913,6 +1149,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1070,13 +1309,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1317625</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1263650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1642,13 +1881,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>146051</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1352551</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1277145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1685,15 +1924,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>69851</xdr:colOff>
+      <xdr:colOff>73026</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>63501</xdr:rowOff>
+      <xdr:rowOff>111126</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1441451</xdr:colOff>
+      <xdr:colOff>1390650</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>1371035</xdr:rowOff>
+      <xdr:rowOff>1367205</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1716,8 +1955,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3282951" y="32423101"/>
-          <a:ext cx="1371600" cy="1307534"/>
+          <a:off x="3400426" y="32064326"/>
+          <a:ext cx="1317624" cy="1256079"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1730,13 +1969,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1397001</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>1367057</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1774,13 +2013,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>158751</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>177801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>1333999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2122,12 +2361,195 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1329717</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1311275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB8B710-B8FB-4510-BD43-5895A44090F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3355976" y="36458525"/>
+          <a:ext cx="1294791" cy="1127125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>88901</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>330200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1368426</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1201854</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2633550C-AF7F-479F-8473-D904C913B3C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3416301" y="38049200"/>
+          <a:ext cx="1276350" cy="871654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>144720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1292224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD8B36C-CB71-450F-AADE-658D07385DA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3419475" y="39305170"/>
+          <a:ext cx="1222375" cy="1137979"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A1:K35" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A1:K35" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A1:K38" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A1:K38" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{8DD10BD1-F8F8-4CF0-8D4C-7F4FC801B3C7}" name="SubAssy"/>
     <tableColumn id="2" xr3:uid="{48F8A639-6252-46BC-8E09-3A18B47C9DCC}" name="Category"/>
@@ -2466,26 +2888,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" customWidth="1"/>
-    <col min="5" max="5" width="42.453125" customWidth="1"/>
-    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="9" max="9" width="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.453125" customWidth="1"/>
-    <col min="11" max="11" width="42.1796875" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" customWidth="1"/>
+    <col min="11" max="11" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2520,7 +2942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>49</v>
       </c>
@@ -2535,7 +2957,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="35"/>
     </row>
-    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>65</v>
       </c>
@@ -2568,7 +2990,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>65</v>
       </c>
@@ -2601,7 +3023,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>65</v>
       </c>
@@ -2634,7 +3056,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
@@ -2667,7 +3089,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>65</v>
       </c>
@@ -2700,7 +3122,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>65</v>
       </c>
@@ -2733,7 +3155,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>59</v>
       </c>
@@ -2748,7 +3170,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="35"/>
     </row>
-    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>65</v>
       </c>
@@ -2775,13 +3197,13 @@
         <v>58</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>65</v>
       </c>
@@ -2806,7 +3228,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>65</v>
       </c>
@@ -2835,7 +3257,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>65</v>
       </c>
@@ -2859,16 +3281,16 @@
         <v>1</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>65</v>
       </c>
@@ -2895,13 +3317,13 @@
         <v>73</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>65</v>
       </c>
@@ -2926,13 +3348,13 @@
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>65</v>
       </c>
@@ -2959,7 +3381,7 @@
       <c r="J16" s="18"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>65</v>
       </c>
@@ -2986,7 +3408,7 @@
       <c r="J17" s="18"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>65</v>
       </c>
@@ -3013,7 +3435,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
     </row>
-    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>65</v>
       </c>
@@ -3040,7 +3462,7 @@
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
     </row>
-    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>65</v>
       </c>
@@ -3067,7 +3489,7 @@
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="1:11" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
         <v>76</v>
       </c>
@@ -3082,7 +3504,7 @@
       <c r="J21" s="49"/>
       <c r="K21" s="46"/>
     </row>
-    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>65</v>
       </c>
@@ -3115,7 +3537,7 @@
       </c>
       <c r="K22" s="17"/>
     </row>
-    <row r="23" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>77</v>
       </c>
@@ -3130,7 +3552,7 @@
       <c r="J23" s="45"/>
       <c r="K23" s="46"/>
     </row>
-    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>65</v>
       </c>
@@ -3163,7 +3585,7 @@
       </c>
       <c r="K24" s="17"/>
     </row>
-    <row r="25" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
         <v>78</v>
       </c>
@@ -3178,263 +3600,350 @@
       <c r="J25" s="45"/>
       <c r="K25" s="46"/>
     </row>
-    <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>79</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F26" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G26" s="23"/>
-      <c r="H26" s="28">
-        <v>1</v>
+      <c r="H26" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="J26" s="25"/>
       <c r="K26" s="30"/>
     </row>
-    <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>80</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F27" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G27" s="23"/>
-      <c r="H27" s="28">
-        <v>1</v>
+      <c r="H27" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="J27" s="25"/>
       <c r="K27" s="30"/>
     </row>
-    <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="24">
-        <v>13</v>
+        <v>108</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="26" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="F28" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G28" s="23"/>
-      <c r="H28" s="28">
-        <v>1</v>
+      <c r="H28" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="J28" s="25"/>
       <c r="K28" s="30"/>
     </row>
-    <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="24">
-        <v>13</v>
+        <v>108</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>100</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="26" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F29" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="23"/>
-      <c r="H29" s="28">
-        <v>1</v>
+      <c r="H29" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="J29" s="25"/>
       <c r="K29" s="30"/>
     </row>
-    <row r="30" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="24">
-        <v>13</v>
+        <v>108</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>101</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="26" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G30" s="23"/>
-      <c r="H30" s="28">
-        <v>1</v>
+      <c r="H30" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="I30" s="29" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="30"/>
     </row>
-    <row r="31" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="38" t="s">
+    <row r="31" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="23"/>
+      <c r="H31" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="K31" s="30"/>
+    </row>
+    <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="23"/>
+      <c r="H32" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="J32" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="K32" s="30"/>
+    </row>
+    <row r="33" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" s="23"/>
+      <c r="H33" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J33" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="K33" s="30"/>
+    </row>
+    <row r="34" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="46"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="46"/>
     </row>
-    <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+    <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="11">
-        <v>11</v>
-      </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="14" t="s">
+      <c r="C35" s="11">
+        <v>14</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="15">
+      <c r="G35" s="10"/>
+      <c r="H35" s="15">
         <v>1</v>
       </c>
-      <c r="I32" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J32" s="12"/>
-      <c r="K32" s="17"/>
+      <c r="I35" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" s="12"/>
+      <c r="K35" s="17"/>
     </row>
-    <row r="33" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    <row r="36" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="11">
-        <v>12</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13" t="s">
+      <c r="C36" s="11">
+        <v>15</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F36" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="15">
+      <c r="G36" s="10"/>
+      <c r="H36" s="15">
         <v>1</v>
       </c>
-      <c r="I33" s="16" t="s">
+      <c r="I36" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J33" s="12"/>
-      <c r="K33" s="17"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="17"/>
     </row>
-    <row r="34" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
+    <row r="37" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="11">
-        <v>13</v>
-      </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="14" t="s">
+      <c r="C37" s="11">
+        <v>16</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="15">
+      <c r="G37" s="10"/>
+      <c r="H37" s="15">
         <v>1</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="I37" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J34" s="12"/>
-      <c r="K34" s="17"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="17"/>
     </row>
-    <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="22" t="s">
+    <row r="38" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="24">
-        <v>13</v>
-      </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="27" t="s">
+      <c r="B38" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="28">
-        <v>1</v>
-      </c>
-      <c r="I35" s="31" t="s">
+      <c r="G38" s="23"/>
+      <c r="H38" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="J35" s="25"/>
-      <c r="K35" s="30"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Link to Thingiverse Added to BOM
</commit_message>
<xml_diff>
--- a/files/HOTEND_EXTRUDER/RAPIDO/BOM_HextrudORT_Extruder_Rapido.xlsx
+++ b/files/HOTEND_EXTRUDER/RAPIDO/BOM_HextrudORT_Extruder_Rapido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\RAPIDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF08969E-8929-4440-A771-6B2C141F9603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3356E6-4C6C-4B70-A2C7-1CCE8E446016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="132">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -645,12 +645,48 @@
   <si>
     <t>USER MOD!! Thanks to DonnerPlays from HevORT Discord channel</t>
   </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173650</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173651</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173652</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173653</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173654</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173655</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173656</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173657</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173659</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173660</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173661</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:5173662</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,6 +853,12 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2890,8 +2932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3667,9 @@
         <v>110</v>
       </c>
       <c r="J26" s="25"/>
-      <c r="K26" s="30"/>
+      <c r="K26" s="30" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -3652,7 +3696,9 @@
         <v>109</v>
       </c>
       <c r="J27" s="25"/>
-      <c r="K27" s="30"/>
+      <c r="K27" s="30" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -3679,7 +3725,9 @@
         <v>107</v>
       </c>
       <c r="J28" s="25"/>
-      <c r="K28" s="30"/>
+      <c r="K28" s="30" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
@@ -3706,7 +3754,9 @@
         <v>112</v>
       </c>
       <c r="J29" s="25"/>
-      <c r="K29" s="30"/>
+      <c r="K29" s="30" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -3733,7 +3783,9 @@
         <v>111</v>
       </c>
       <c r="J30" s="25"/>
-      <c r="K30" s="30"/>
+      <c r="K30" s="30" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
@@ -3762,7 +3814,9 @@
       <c r="J31" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="K31" s="30"/>
+      <c r="K31" s="30" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -3791,7 +3845,9 @@
       <c r="J32" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="K32" s="30"/>
+      <c r="K32" s="30" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
@@ -3820,7 +3876,9 @@
       <c r="J33" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="K33" s="30"/>
+      <c r="K33" s="30" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
@@ -3835,7 +3893,7 @@
       <c r="H34" s="43"/>
       <c r="I34" s="44"/>
       <c r="J34" s="45"/>
-      <c r="K34" s="46"/>
+      <c r="K34" s="45"/>
     </row>
     <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
@@ -3862,7 +3920,9 @@
         <v>95</v>
       </c>
       <c r="J35" s="12"/>
-      <c r="K35" s="17"/>
+      <c r="K35" s="30" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
@@ -3889,7 +3949,9 @@
         <v>32</v>
       </c>
       <c r="J36" s="12"/>
-      <c r="K36" s="17"/>
+      <c r="K36" s="30" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
@@ -3916,7 +3978,9 @@
         <v>33</v>
       </c>
       <c r="J37" s="12"/>
-      <c r="K37" s="17"/>
+      <c r="K37" s="30" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
@@ -3943,9 +4007,12 @@
         <v>82</v>
       </c>
       <c r="J38" s="25"/>
-      <c r="K38" s="30"/>
+      <c r="K38" s="30" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="22" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{48E6D9EF-D3CC-4632-AF5B-F066AE980C97}"/>
     <hyperlink ref="K4" r:id="rId2" xr:uid="{ED13E1FE-81C8-412D-BCE7-9AF106557271}"/>

</xml_diff>

<commit_message>
Rapido 1.65 BOM Update
</commit_message>
<xml_diff>
--- a/files/HOTEND_EXTRUDER/RAPIDO/BOM_HextrudORT_Extruder_Rapido.xlsx
+++ b/files/HOTEND_EXTRUDER/RAPIDO/BOM_HextrudORT_Extruder_Rapido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\RAPIDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A905E-61B5-43C9-B47D-59A2803274F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6DED0C-02CA-4FA6-B589-458B03BA7F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="118">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -511,9 +511,6 @@
     <t>HextrudORT/files/HOTEND_EXTRUDER/RAPIDO/STLs at main · MirageC79/HextrudORT (github.com)</t>
   </si>
   <si>
-    <t xml:space="preserve">V1.65 integrates a few changes to accept the new RIDGA gear from Bondtech as well as some enhancement to the overal rigidity of the unit.   </t>
-  </si>
-  <si>
     <t>https://s.click.aliexpress.com/e/_DEoG91j</t>
   </si>
   <si>
@@ -596,6 +593,22 @@
   </si>
   <si>
     <t>HextrudORT_COVER_MR84_V1.65_RIDGA</t>
+  </si>
+  <si>
+    <t>18d</t>
+  </si>
+  <si>
+    <t>HextrudORT_STDHT_MGN9_RapidoUHF_StructFanShroud_25mm_BLTouch v1.stl</t>
+  </si>
+  <si>
+    <t>*OPTION
+Allows the mounting of Bltouch directly onto the FanShroud</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.65 integrates a few changes to accept the new RIDGA gear from Bondtech as well as some enhancements to the overal rigidity of the unit.   </t>
   </si>
 </sst>
 </file>
@@ -1161,9 +1174,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1198,6 +1208,9 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1205,6 +1218,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1238,13 +1258,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1706,13 +1719,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>73026</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>111126</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1390650</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>1367205</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1750,13 +1763,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1397001</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1367057</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1926,13 +1939,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>114301</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1366595</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>1346201</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1970,13 +1983,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>95251</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>120651</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1377951</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>1343437</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2014,13 +2027,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>120651</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>177801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1359621</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1358900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2058,13 +2071,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>88901</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>101601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1394483</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1346200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2102,13 +2115,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1329717</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>1311275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2163,13 +2176,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>88901</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>330200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1368426</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>1201854</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2224,13 +2237,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>92075</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>144720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1314450</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1292224</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2373,13 +2386,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>158751</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1244601</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>1349261</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2417,13 +2430,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>86528</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>318895</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1393608</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>1594478</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2461,13 +2474,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>273538</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>53731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266447</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>1376216</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2633,12 +2646,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>90715</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>281216</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1360715</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1139042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE841BAD-A880-DFD6-B2C5-AEF53D8A9B74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3546929" y="30552573"/>
+          <a:ext cx="1270000" cy="857826"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A2:K39" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
-  <autoFilter ref="A2:K39" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A2:K40" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A2:K40" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{8DD10BD1-F8F8-4CF0-8D4C-7F4FC801B3C7}" name="SubAssy"/>
     <tableColumn id="2" xr3:uid="{48F8A639-6252-46BC-8E09-3A18B47C9DCC}" name="Category"/>
@@ -2977,10 +3034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3001,56 +3058,56 @@
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="45"/>
-      <c r="E1" s="57" t="str">
+      <c r="E1" s="56" t="str">
         <f>HYPERLINK("https://a360.co/3JzDvPC","LINK TO CAD")</f>
         <v>LINK TO CAD</v>
       </c>
-      <c r="F1" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
+      <c r="F1" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="24"/>
@@ -3091,7 +3148,7 @@
       <c r="J4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="K4" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3122,7 +3179,7 @@
       <c r="J5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="K5" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3153,7 +3210,7 @@
       <c r="J6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="56" t="s">
+      <c r="K6" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3184,7 +3241,7 @@
       <c r="J7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="56" t="s">
+      <c r="K7" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3215,7 +3272,7 @@
       <c r="J8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="56" t="s">
+      <c r="K8" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3246,7 +3303,7 @@
       <c r="J9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="55" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3428,10 +3485,10 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>28</v>
@@ -3439,14 +3496,14 @@
       <c r="H16" s="8">
         <v>3</v>
       </c>
-      <c r="I16" s="58" t="s">
-        <v>96</v>
+      <c r="I16" s="57" t="s">
+        <v>95</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>59</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3488,10 +3545,10 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>28</v>
@@ -3500,7 +3557,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="10"/>
@@ -3529,7 +3586,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="10"/>
@@ -3558,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="10"/>
@@ -3587,7 +3644,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="10"/>
@@ -3615,7 +3672,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>22</v>
@@ -3640,99 +3697,101 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="39" t="s">
+    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" s="55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="38"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="38"/>
     </row>
-    <row r="25" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="C26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K25" s="10"/>
+      <c r="K26" s="10"/>
     </row>
-    <row r="26" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
+    <row r="27" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
-    </row>
-    <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="J27" s="18"/>
-      <c r="K27" s="56" t="s">
-        <v>92</v>
-      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
@@ -3742,11 +3801,11 @@
         <v>70</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>6</v>
@@ -3758,10 +3817,10 @@
         <v>23</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J28" s="18"/>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3773,11 +3832,11 @@
         <v>70</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="18"/>
-      <c r="E29" s="19" t="s">
-        <v>66</v>
+      <c r="E29" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>6</v>
@@ -3789,10 +3848,10 @@
         <v>23</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J29" s="18"/>
-      <c r="K29" s="56" t="s">
+      <c r="K29" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3804,11 +3863,11 @@
         <v>70</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>6</v>
@@ -3820,10 +3879,10 @@
         <v>23</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J30" s="18"/>
-      <c r="K30" s="56" t="s">
+      <c r="K30" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3835,14 +3894,14 @@
         <v>70</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>15</v>
@@ -3851,10 +3910,10 @@
         <v>23</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J31" s="18"/>
-      <c r="K31" s="56" t="s">
+      <c r="K31" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3866,14 +3925,14 @@
         <v>70</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="19" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>15</v>
@@ -3882,12 +3941,10 @@
         <v>23</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="J32" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="K32" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3899,11 +3956,11 @@
         <v>70</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>6</v>
@@ -3915,12 +3972,12 @@
         <v>23</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J33" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="K33" s="56" t="s">
+      <c r="K33" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3936,10 +3993,10 @@
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>15</v>
@@ -3948,89 +4005,91 @@
         <v>23</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J34" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="K34" s="56" t="s">
+      <c r="K34" s="55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="30" t="s">
+    <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="K35" s="55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-    </row>
-    <row r="36" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="56" t="s">
-        <v>92</v>
-      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
     </row>
     <row r="37" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="4">
-        <v>21</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>5</v>
+      <c r="B37" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>6</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="8">
-        <v>1</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J37" s="5"/>
-      <c r="K37" s="56" t="s">
+      <c r="H37" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" s="18"/>
+      <c r="K37" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4042,11 +4101,11 @@
         <v>15</v>
       </c>
       <c r="C38" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>5</v>
@@ -4057,13 +4116,15 @@
       <c r="H38" s="8">
         <v>1</v>
       </c>
-      <c r="I38" s="9"/>
+      <c r="I38" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="J38" s="5"/>
-      <c r="K38" s="56" t="s">
+      <c r="K38" s="55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -4071,14 +4132,14 @@
         <v>15</v>
       </c>
       <c r="C39" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6" t="s">
         <v>112</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>15</v>
@@ -4086,11 +4147,40 @@
       <c r="H39" s="8">
         <v>1</v>
       </c>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="9"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="4">
+        <v>23</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="56" t="s">
+      <c r="J40" s="5"/>
+      <c r="K40" s="55" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4102,20 +4192,21 @@
   <hyperlinks>
     <hyperlink ref="K4" r:id="rId1" display="https://www.bondtech.se/product/bmg-reverse-set-for-hextrudort/" xr:uid="{90E87D2C-E3BF-4A14-B0DB-F93FEA30ADB6}"/>
     <hyperlink ref="K5:K9" r:id="rId2" display="https://www.bondtech.se/product/bmg-reverse-set-for-hextrudort/" xr:uid="{4EEC4F7B-4CBD-4636-89B4-2FD3EC6706EE}"/>
-    <hyperlink ref="K39" r:id="rId3" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{8C117F71-DCB4-402F-9BF5-AD25D21836F8}"/>
-    <hyperlink ref="K37:K38" r:id="rId4" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{29D6726E-D3E0-4865-BE25-111E1FA08715}"/>
-    <hyperlink ref="K34" r:id="rId5" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{FFEF7BF7-6AFB-405B-B5C3-44C536D9D610}"/>
-    <hyperlink ref="K27:K33" r:id="rId6" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{AA5892DB-A442-4A4D-882B-1D3CF7B54909}"/>
+    <hyperlink ref="K40" r:id="rId3" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{8C117F71-DCB4-402F-9BF5-AD25D21836F8}"/>
+    <hyperlink ref="K38:K39" r:id="rId4" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{29D6726E-D3E0-4865-BE25-111E1FA08715}"/>
+    <hyperlink ref="K35" r:id="rId5" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{FFEF7BF7-6AFB-405B-B5C3-44C536D9D610}"/>
+    <hyperlink ref="K28:K34" r:id="rId6" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{AA5892DB-A442-4A4D-882B-1D3CF7B54909}"/>
     <hyperlink ref="K16" r:id="rId7" xr:uid="{46B43DC0-12D7-45C6-80DC-9AAE94DD6860}"/>
+    <hyperlink ref="K24" r:id="rId8" display="https://github.com/MirageC79/HextrudORT/tree/main/files/HOTEND_EXTRUDER/RAPIDO/STLs" xr:uid="{4E0FB65B-426B-4B0A-84F8-F1562731F0B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <drawing r:id="rId10"/>
   <webPublishItems count="1">
     <webPublishItem id="24158" divId="BOM_HextrudORT_Extruder_Dragon_24158" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\RAPIDO\BOM_HextrudORT_Extruder_Rapido.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>